<commit_message>
Final day updates (~2 hours of work)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">Phase</t>
   </si>
@@ -144,124 +144,187 @@
     <t xml:space="preserve">OGA.BWD_LF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.BWD_LF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.BWD_LF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.BWD_LH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.BWD_LH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.BWD_LH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.BWD_RF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.BWD_RF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.BWD_RF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.BWD_RH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.BWD_RH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.BWD_RH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.BWD_AL.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.BWD_AL.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.BWD_AL.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.PVF_LF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.PVF_LF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.PVF_LF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.PVF_LH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.PVF_LH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.PVF_LH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.PVF_RF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.PVF_RF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.PVF_RF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.PVF_RH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.PVF_RH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.PVF_RH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.PVF_AL.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.PVF_AL.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.PVF_AL.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.VI_LF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.VI_LF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.VI_LF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.VI_LH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.VI_LH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.VI_LH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.VI_RF.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.VI_RF.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.VI_RF.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.VI_RH.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.VI_RH.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.VI_RH.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">OGA.VI_AL.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">OGA.VI_AL.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">OGA.VI_AL.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">SOS.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">SOS.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOS.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">CSOM.ACT(MEAN).Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">CSOM.ACT(MEAN).Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSOM.ACT(MEAN).Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">CSOM.BEHAV(MEAN).Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">CSOM.BEHAV(MEAN).Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSOM.BEHAV(MEAN).Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">CBPI.PSS.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">CBPI.PSS.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">CBPI.PSS.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">CBPI.PIS.Phase</t>
   </si>
   <si>
+    <t xml:space="preserve">CBPI.PIS.Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">CBPI.PIS.Phase:Group</t>
   </si>
   <si>
     <t xml:space="preserve">CBPI.QOL.Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBPI.QOL.Group</t>
   </si>
   <si>
     <t xml:space="preserve">CBPI.QOL.Phase:Group</t>
@@ -4725,22 +4788,22 @@
         <v>43</v>
       </c>
       <c r="B3" t="n">
-        <v>17.7391769501674</v>
+        <v>5.53294211058982</v>
       </c>
       <c r="C3" t="n">
-        <v>8.86958847508371</v>
+        <v>5.53294211058982</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>167.374651763064</v>
+        <v>38.1922517408941</v>
       </c>
       <c r="F3" t="n">
-        <v>3.19208146686091</v>
+        <v>1.99125382401254</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0435995335618908</v>
+        <v>0.166304387932657</v>
       </c>
     </row>
     <row r="4">
@@ -4748,22 +4811,22 @@
         <v>44</v>
       </c>
       <c r="B4" t="n">
-        <v>1.56090520942153</v>
+        <v>17.7391769501674</v>
       </c>
       <c r="C4" t="n">
-        <v>0.780452604710767</v>
+        <v>8.86958847508371</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>166.580064604797</v>
+        <v>167.374651763064</v>
       </c>
       <c r="F4" t="n">
-        <v>0.409904482627128</v>
+        <v>3.19208146686091</v>
       </c>
       <c r="G4" t="n">
-        <v>0.664381248017616</v>
+        <v>0.0435995335618908</v>
       </c>
     </row>
     <row r="5">
@@ -4771,22 +4834,22 @@
         <v>45</v>
       </c>
       <c r="B5" t="n">
-        <v>3.45884927661183</v>
+        <v>1.56090520942153</v>
       </c>
       <c r="C5" t="n">
-        <v>1.72942463830592</v>
+        <v>0.780452604710767</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>166.580064603455</v>
+        <v>166.580064604797</v>
       </c>
       <c r="F5" t="n">
-        <v>0.908317695819734</v>
+        <v>0.409904482627128</v>
       </c>
       <c r="G5" t="n">
-        <v>0.405189430068027</v>
+        <v>0.664381248017616</v>
       </c>
     </row>
     <row r="6">
@@ -4794,22 +4857,22 @@
         <v>46</v>
       </c>
       <c r="B6" t="n">
-        <v>0.298603583032243</v>
+        <v>2.59312217503302</v>
       </c>
       <c r="C6" t="n">
-        <v>0.149301791516122</v>
+        <v>2.59312217503302</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>166.200731313044</v>
+        <v>37.6070903739324</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0398794489169723</v>
+        <v>1.36194356598984</v>
       </c>
       <c r="G6" t="n">
-        <v>0.960914462322098</v>
+        <v>0.250547734804832</v>
       </c>
     </row>
     <row r="7">
@@ -4817,22 +4880,22 @@
         <v>47</v>
       </c>
       <c r="B7" t="n">
-        <v>2.81789872106875</v>
+        <v>3.45884927661183</v>
       </c>
       <c r="C7" t="n">
-        <v>1.40894936053438</v>
+        <v>1.72942463830592</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>166.200731318644</v>
+        <v>166.580064603455</v>
       </c>
       <c r="F7" t="n">
-        <v>0.376339248708642</v>
+        <v>0.908317695819734</v>
       </c>
       <c r="G7" t="n">
-        <v>0.686952834701926</v>
+        <v>0.405189430068027</v>
       </c>
     </row>
     <row r="8">
@@ -4840,22 +4903,22 @@
         <v>48</v>
       </c>
       <c r="B8" t="n">
-        <v>6.62387001561929</v>
+        <v>0.298603583032243</v>
       </c>
       <c r="C8" t="n">
-        <v>3.31193500780965</v>
+        <v>0.149301791516122</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>166.732949735225</v>
+        <v>166.200731313044</v>
       </c>
       <c r="F8" t="n">
-        <v>1.24972823594646</v>
+        <v>0.0398794489169723</v>
       </c>
       <c r="G8" t="n">
-        <v>0.289252979660829</v>
+        <v>0.960914462322098</v>
       </c>
     </row>
     <row r="9">
@@ -4863,22 +4926,22 @@
         <v>49</v>
       </c>
       <c r="B9" t="n">
-        <v>17.8230483275453</v>
+        <v>0.0164546236030566</v>
       </c>
       <c r="C9" t="n">
-        <v>8.91152416377267</v>
+        <v>0.0164546236030566</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>166.732949734448</v>
+        <v>37.4495006231142</v>
       </c>
       <c r="F9" t="n">
-        <v>3.36268173938332</v>
+        <v>0.00439513360665365</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0370075552706927</v>
+        <v>0.94749499185026</v>
       </c>
     </row>
     <row r="10">
@@ -4886,22 +4949,22 @@
         <v>50</v>
       </c>
       <c r="B10" t="n">
-        <v>11.7582699732846</v>
+        <v>2.81789872106875</v>
       </c>
       <c r="C10" t="n">
-        <v>5.87913498664228</v>
+        <v>1.40894936053438</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>166.618259445827</v>
+        <v>166.200731318644</v>
       </c>
       <c r="F10" t="n">
-        <v>2.08886617135532</v>
+        <v>0.376339248708642</v>
       </c>
       <c r="G10" t="n">
-        <v>0.127058448625332</v>
+        <v>0.686952834701926</v>
       </c>
     </row>
     <row r="11">
@@ -4909,22 +4972,22 @@
         <v>51</v>
       </c>
       <c r="B11" t="n">
-        <v>1.65465537459672</v>
+        <v>6.62387001561929</v>
       </c>
       <c r="C11" t="n">
-        <v>0.827327687298358</v>
+        <v>3.31193500780965</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>166.61825944534</v>
+        <v>166.732949735225</v>
       </c>
       <c r="F11" t="n">
-        <v>0.293950865654503</v>
+        <v>1.24972823594646</v>
       </c>
       <c r="G11" t="n">
-        <v>0.745698818368893</v>
+        <v>0.289252979660829</v>
       </c>
     </row>
     <row r="12">
@@ -4932,22 +4995,22 @@
         <v>52</v>
       </c>
       <c r="B12" t="n">
-        <v>210.809904126563</v>
+        <v>0.262294723751476</v>
       </c>
       <c r="C12" t="n">
-        <v>105.404952063281</v>
+        <v>0.262294723751476</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>166.817482543434</v>
+        <v>36.8274927059749</v>
       </c>
       <c r="F12" t="n">
-        <v>0.435855892924597</v>
+        <v>0.0989745033157474</v>
       </c>
       <c r="G12" t="n">
-        <v>0.647445244816202</v>
+        <v>0.754839272786561</v>
       </c>
     </row>
     <row r="13">
@@ -4955,22 +5018,22 @@
         <v>53</v>
       </c>
       <c r="B13" t="n">
-        <v>76.8939188961057</v>
+        <v>17.8230483275453</v>
       </c>
       <c r="C13" t="n">
-        <v>38.4469594480528</v>
+        <v>8.91152416377267</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>166.81748254984</v>
+        <v>166.732949734448</v>
       </c>
       <c r="F13" t="n">
-        <v>0.158980517636461</v>
+        <v>3.36268173938332</v>
       </c>
       <c r="G13" t="n">
-        <v>0.853142064760604</v>
+        <v>0.0370075552706927</v>
       </c>
     </row>
     <row r="14">
@@ -4978,22 +5041,22 @@
         <v>54</v>
       </c>
       <c r="B14" t="n">
-        <v>59.6478277920736</v>
+        <v>11.7582699732846</v>
       </c>
       <c r="C14" t="n">
-        <v>29.8239138960368</v>
+        <v>5.87913498664228</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>166.873977228903</v>
+        <v>166.618259445827</v>
       </c>
       <c r="F14" t="n">
-        <v>0.270751534837731</v>
+        <v>2.08886617135532</v>
       </c>
       <c r="G14" t="n">
-        <v>0.763140448247738</v>
+        <v>0.127058448625332</v>
       </c>
     </row>
     <row r="15">
@@ -5001,22 +5064,22 @@
         <v>55</v>
       </c>
       <c r="B15" t="n">
-        <v>178.871258931889</v>
+        <v>12.3569433594248</v>
       </c>
       <c r="C15" t="n">
-        <v>89.4356294659445</v>
+        <v>12.3569433594248</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>166.873977222064</v>
+        <v>38.0224966567656</v>
       </c>
       <c r="F15" t="n">
-        <v>0.811926765598023</v>
+        <v>4.39044196527252</v>
       </c>
       <c r="G15" t="n">
-        <v>0.445747883148876</v>
+        <v>0.0428540655690654</v>
       </c>
     </row>
     <row r="16">
@@ -5024,22 +5087,22 @@
         <v>56</v>
       </c>
       <c r="B16" t="n">
-        <v>88.0587797275167</v>
+        <v>1.65465537459672</v>
       </c>
       <c r="C16" t="n">
-        <v>44.0293898637583</v>
+        <v>0.827327687298358</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>166.147428808311</v>
+        <v>166.61825944534</v>
       </c>
       <c r="F16" t="n">
-        <v>0.189504182966078</v>
+        <v>0.293950865654503</v>
       </c>
       <c r="G16" t="n">
-        <v>0.827547835031855</v>
+        <v>0.745698818368893</v>
       </c>
     </row>
     <row r="17">
@@ -5047,22 +5110,22 @@
         <v>57</v>
       </c>
       <c r="B17" t="n">
-        <v>31.8264527618865</v>
+        <v>210.809904126563</v>
       </c>
       <c r="C17" t="n">
-        <v>15.9132263809432</v>
+        <v>105.404952063281</v>
       </c>
       <c r="D17" t="n">
         <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>166.147428800853</v>
+        <v>166.817482543434</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0684911367840033</v>
+        <v>0.435855892924597</v>
       </c>
       <c r="G17" t="n">
-        <v>0.933828087565697</v>
+        <v>0.647445244816202</v>
       </c>
     </row>
     <row r="18">
@@ -5070,22 +5133,22 @@
         <v>58</v>
       </c>
       <c r="B18" t="n">
-        <v>160.970911140054</v>
+        <v>444.579345474953</v>
       </c>
       <c r="C18" t="n">
-        <v>80.4854555700269</v>
+        <v>444.579345474953</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>166.232554560188</v>
+        <v>37.1945989698594</v>
       </c>
       <c r="F18" t="n">
-        <v>0.752266129551026</v>
+        <v>1.83836265568894</v>
       </c>
       <c r="G18" t="n">
-        <v>0.472894840822775</v>
+        <v>0.1833183598272</v>
       </c>
     </row>
     <row r="19">
@@ -5093,22 +5156,22 @@
         <v>59</v>
       </c>
       <c r="B19" t="n">
-        <v>533.142481930331</v>
+        <v>76.8939188961057</v>
       </c>
       <c r="C19" t="n">
-        <v>266.571240965165</v>
+        <v>38.4469594480528</v>
       </c>
       <c r="D19" t="n">
         <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>166.232554561427</v>
+        <v>166.81748254984</v>
       </c>
       <c r="F19" t="n">
-        <v>2.49153731280063</v>
+        <v>0.158980517636461</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0858697726940102</v>
+        <v>0.853142064760604</v>
       </c>
     </row>
     <row r="20">
@@ -5116,22 +5179,22 @@
         <v>60</v>
       </c>
       <c r="B20" t="n">
-        <v>365.328592038847</v>
+        <v>59.6478277920736</v>
       </c>
       <c r="C20" t="n">
-        <v>182.664296019424</v>
+        <v>29.8239138960368</v>
       </c>
       <c r="D20" t="n">
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>165.886275683691</v>
+        <v>166.873977228903</v>
       </c>
       <c r="F20" t="n">
-        <v>1.47680636191878</v>
+        <v>0.270751534837731</v>
       </c>
       <c r="G20" t="n">
-        <v>0.231352429177888</v>
+        <v>0.763140448247738</v>
       </c>
     </row>
     <row r="21">
@@ -5139,22 +5202,22 @@
         <v>61</v>
       </c>
       <c r="B21" t="n">
-        <v>185.275094848832</v>
+        <v>0.225052567448228</v>
       </c>
       <c r="C21" t="n">
-        <v>92.6375474244161</v>
+        <v>0.225052567448228</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>165.886275687967</v>
+        <v>37.1384972872444</v>
       </c>
       <c r="F21" t="n">
-        <v>0.748957088879499</v>
+        <v>0.00204310300345512</v>
       </c>
       <c r="G21" t="n">
-        <v>0.474451511690213</v>
+        <v>0.96418951330352</v>
       </c>
     </row>
     <row r="22">
@@ -5162,22 +5225,22 @@
         <v>62</v>
       </c>
       <c r="B22" t="n">
-        <v>5.22353360829561</v>
+        <v>178.871258931889</v>
       </c>
       <c r="C22" t="n">
-        <v>2.6117668041478</v>
+        <v>89.4356294659445</v>
       </c>
       <c r="D22" t="n">
         <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>163.240805960733</v>
+        <v>166.873977222064</v>
       </c>
       <c r="F22" t="n">
-        <v>0.244450813216406</v>
+        <v>0.811926765598023</v>
       </c>
       <c r="G22" t="n">
-        <v>0.783420663962289</v>
+        <v>0.445747883148876</v>
       </c>
     </row>
     <row r="23">
@@ -5185,22 +5248,22 @@
         <v>63</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0111347804014</v>
+        <v>88.0587797275167</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0055673902007</v>
+        <v>44.0293898637583</v>
       </c>
       <c r="D23" t="n">
         <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>163.240805956427</v>
+        <v>166.147428808311</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0941170421065472</v>
+        <v>0.189504182966078</v>
       </c>
       <c r="G23" t="n">
-        <v>0.910225579815204</v>
+        <v>0.827547835031855</v>
       </c>
     </row>
     <row r="24">
@@ -5208,22 +5271,22 @@
         <v>64</v>
       </c>
       <c r="B24" t="n">
-        <v>0.226236755016789</v>
+        <v>71.3745906545751</v>
       </c>
       <c r="C24" t="n">
-        <v>0.113118377508395</v>
+        <v>71.3745906545751</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>165.78205756343</v>
+        <v>36.9712446729824</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0384780997550444</v>
+        <v>0.307198976147224</v>
       </c>
       <c r="G24" t="n">
-        <v>0.96226136913454</v>
+        <v>0.582741487314742</v>
       </c>
     </row>
     <row r="25">
@@ -5231,22 +5294,22 @@
         <v>65</v>
       </c>
       <c r="B25" t="n">
-        <v>1.27460864315939</v>
+        <v>31.8264527618865</v>
       </c>
       <c r="C25" t="n">
-        <v>0.637304321579695</v>
+        <v>15.9132263809432</v>
       </c>
       <c r="D25" t="n">
         <v>2</v>
       </c>
       <c r="E25" t="n">
-        <v>165.782057558576</v>
+        <v>166.147428800853</v>
       </c>
       <c r="F25" t="n">
-        <v>0.216784043408372</v>
+        <v>0.0684911367840033</v>
       </c>
       <c r="G25" t="n">
-        <v>0.805331681137442</v>
+        <v>0.933828087565697</v>
       </c>
     </row>
     <row r="26">
@@ -5254,22 +5317,22 @@
         <v>66</v>
       </c>
       <c r="B26" t="n">
-        <v>10.9123228898989</v>
+        <v>160.970911140054</v>
       </c>
       <c r="C26" t="n">
-        <v>5.45616144494945</v>
+        <v>80.4854555700269</v>
       </c>
       <c r="D26" t="n">
         <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>159.61334026248</v>
+        <v>166.232554560188</v>
       </c>
       <c r="F26" t="n">
-        <v>0.479013990680857</v>
+        <v>0.752266129551026</v>
       </c>
       <c r="G26" t="n">
-        <v>0.620281325417251</v>
+        <v>0.472894840822775</v>
       </c>
     </row>
     <row r="27">
@@ -5277,22 +5340,22 @@
         <v>67</v>
       </c>
       <c r="B27" t="n">
-        <v>3.61364070958892</v>
+        <v>29.1137085866116</v>
       </c>
       <c r="C27" t="n">
-        <v>1.80682035479446</v>
+        <v>29.1137085866116</v>
       </c>
       <c r="D27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>159.613340262045</v>
+        <v>36.545668062798</v>
       </c>
       <c r="F27" t="n">
-        <v>0.15862657975318</v>
+        <v>0.272114467393074</v>
       </c>
       <c r="G27" t="n">
-        <v>0.853449298766526</v>
+        <v>0.605064179693335</v>
       </c>
     </row>
     <row r="28">
@@ -5300,22 +5363,22 @@
         <v>68</v>
       </c>
       <c r="B28" t="n">
-        <v>5.76889793299689</v>
+        <v>533.142481930331</v>
       </c>
       <c r="C28" t="n">
-        <v>2.88444896649845</v>
+        <v>266.571240965165</v>
       </c>
       <c r="D28" t="n">
         <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>165.431462258882</v>
+        <v>166.232554561427</v>
       </c>
       <c r="F28" t="n">
-        <v>0.713957089894244</v>
+        <v>2.49153731280063</v>
       </c>
       <c r="G28" t="n">
-        <v>0.491205128149826</v>
+        <v>0.0858697726940102</v>
       </c>
     </row>
     <row r="29">
@@ -5323,22 +5386,22 @@
         <v>69</v>
       </c>
       <c r="B29" t="n">
-        <v>5.73612839020968</v>
+        <v>365.328592038847</v>
       </c>
       <c r="C29" t="n">
-        <v>2.86806419510484</v>
+        <v>182.664296019424</v>
       </c>
       <c r="D29" t="n">
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>165.431462267043</v>
+        <v>165.886275683691</v>
       </c>
       <c r="F29" t="n">
-        <v>0.709901541039461</v>
+        <v>1.47680636191878</v>
       </c>
       <c r="G29" t="n">
-        <v>0.49318421114143</v>
+        <v>0.231352429177888</v>
       </c>
     </row>
     <row r="30">
@@ -5346,22 +5409,22 @@
         <v>70</v>
       </c>
       <c r="B30" t="n">
-        <v>1.97257890977619</v>
+        <v>83.4980578423581</v>
       </c>
       <c r="C30" t="n">
-        <v>0.986289454888094</v>
+        <v>83.4980578423581</v>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>166.368454156484</v>
+        <v>36.7895890512948</v>
       </c>
       <c r="F30" t="n">
-        <v>0.265348731221794</v>
+        <v>0.675066040362615</v>
       </c>
       <c r="G30" t="n">
-        <v>0.767262409098309</v>
+        <v>0.416583914256639</v>
       </c>
     </row>
     <row r="31">
@@ -5369,22 +5432,22 @@
         <v>71</v>
       </c>
       <c r="B31" t="n">
-        <v>0.775013488375225</v>
+        <v>185.275094848832</v>
       </c>
       <c r="C31" t="n">
-        <v>0.387506744187613</v>
+        <v>92.6375474244161</v>
       </c>
       <c r="D31" t="n">
         <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>166.368454153572</v>
+        <v>165.886275687967</v>
       </c>
       <c r="F31" t="n">
-        <v>0.104253799328857</v>
+        <v>0.748957088879499</v>
       </c>
       <c r="G31" t="n">
-        <v>0.901055410980795</v>
+        <v>0.474451511690213</v>
       </c>
     </row>
     <row r="32">
@@ -5392,22 +5455,22 @@
         <v>72</v>
       </c>
       <c r="B32" t="n">
-        <v>4.2644309719298</v>
+        <v>5.22353360829561</v>
       </c>
       <c r="C32" t="n">
-        <v>2.1322154859649</v>
+        <v>2.6117668041478</v>
       </c>
       <c r="D32" t="n">
         <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>166.999605964416</v>
+        <v>163.240805960733</v>
       </c>
       <c r="F32" t="n">
-        <v>1.51921012405298</v>
+        <v>0.244450813216406</v>
       </c>
       <c r="G32" t="n">
-        <v>0.221894082947909</v>
+        <v>0.783420663962289</v>
       </c>
     </row>
     <row r="33">
@@ -5415,22 +5478,22 @@
         <v>73</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0408831236320545</v>
+        <v>46.8788316813471</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0204415618160272</v>
+        <v>46.8788316813471</v>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>166.999605970694</v>
+        <v>33.4415539547588</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0145646759751911</v>
+        <v>4.38766910925629</v>
       </c>
       <c r="G33" t="n">
-        <v>0.985542127583754</v>
+        <v>0.043852753956417</v>
       </c>
     </row>
     <row r="34">
@@ -5438,22 +5501,22 @@
         <v>74</v>
       </c>
       <c r="B34" t="n">
-        <v>1.65201519382752</v>
+        <v>2.0111347804014</v>
       </c>
       <c r="C34" t="n">
-        <v>0.82600759691376</v>
+        <v>1.0055673902007</v>
       </c>
       <c r="D34" t="n">
         <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>167.381180361829</v>
+        <v>163.240805956427</v>
       </c>
       <c r="F34" t="n">
-        <v>4.34988215812931</v>
+        <v>0.0941170421065472</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0143988293435929</v>
+        <v>0.910225579815204</v>
       </c>
     </row>
     <row r="35">
@@ -5461,22 +5524,22 @@
         <v>75</v>
       </c>
       <c r="B35" t="n">
-        <v>0.24578226944085</v>
+        <v>0.226236755016789</v>
       </c>
       <c r="C35" t="n">
-        <v>0.122891134720425</v>
+        <v>0.113118377508395</v>
       </c>
       <c r="D35" t="n">
         <v>2</v>
       </c>
       <c r="E35" t="n">
-        <v>167.381180362697</v>
+        <v>165.78205756343</v>
       </c>
       <c r="F35" t="n">
-        <v>0.647163484101047</v>
+        <v>0.0384780997550444</v>
       </c>
       <c r="G35" t="n">
-        <v>0.524833550797446</v>
+        <v>0.96226136913454</v>
       </c>
     </row>
     <row r="36">
@@ -5484,22 +5547,22 @@
         <v>76</v>
       </c>
       <c r="B36" t="n">
-        <v>3.75470464974175</v>
+        <v>0.387234709779484</v>
       </c>
       <c r="C36" t="n">
-        <v>1.87735232487088</v>
+        <v>0.387234709779484</v>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>166.749929210979</v>
+        <v>36.0744887301008</v>
       </c>
       <c r="F36" t="n">
-        <v>7.3342621111996</v>
+        <v>0.131720911488541</v>
       </c>
       <c r="G36" t="n">
-        <v>0.000885439303093956</v>
+        <v>0.718772347789513</v>
       </c>
     </row>
     <row r="37">
@@ -5507,22 +5570,22 @@
         <v>77</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0346290995055498</v>
+        <v>1.27460864315939</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0173145497527749</v>
+        <v>0.637304321579695</v>
       </c>
       <c r="D37" t="n">
         <v>2</v>
       </c>
       <c r="E37" t="n">
-        <v>166.749929206417</v>
+        <v>165.782057558576</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0676428417521424</v>
+        <v>0.216784043408372</v>
       </c>
       <c r="G37" t="n">
-        <v>0.934619843401819</v>
+        <v>0.805331681137442</v>
       </c>
     </row>
     <row r="38">
@@ -5530,22 +5593,22 @@
         <v>78</v>
       </c>
       <c r="B38" t="n">
-        <v>8.45322707076706</v>
+        <v>10.9123228898989</v>
       </c>
       <c r="C38" t="n">
-        <v>4.22661353538353</v>
+        <v>5.45616144494945</v>
       </c>
       <c r="D38" t="n">
         <v>2</v>
       </c>
       <c r="E38" t="n">
-        <v>167.121558215257</v>
+        <v>159.61334026248</v>
       </c>
       <c r="F38" t="n">
-        <v>5.13473139839836</v>
+        <v>0.479013990680857</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0068524559615141</v>
+        <v>0.620281325417251</v>
       </c>
     </row>
     <row r="39">
@@ -5553,22 +5616,22 @@
         <v>79</v>
       </c>
       <c r="B39" t="n">
-        <v>0.948644424324568</v>
+        <v>52.4623395175316</v>
       </c>
       <c r="C39" t="n">
-        <v>0.474322212162284</v>
+        <v>52.4623395175316</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>167.121558214899</v>
+        <v>30.1874679829216</v>
       </c>
       <c r="F39" t="n">
-        <v>0.576233699948733</v>
+        <v>4.60583779756167</v>
       </c>
       <c r="G39" t="n">
-        <v>0.563123711755617</v>
+        <v>0.0400208144678743</v>
       </c>
     </row>
     <row r="40">
@@ -5576,22 +5639,22 @@
         <v>80</v>
       </c>
       <c r="B40" t="n">
-        <v>12.962952433057</v>
+        <v>3.61364070958892</v>
       </c>
       <c r="C40" t="n">
-        <v>6.4814762165285</v>
+        <v>1.80682035479446</v>
       </c>
       <c r="D40" t="n">
         <v>2</v>
       </c>
       <c r="E40" t="n">
-        <v>166.482583821998</v>
+        <v>159.613340262045</v>
       </c>
       <c r="F40" t="n">
-        <v>7.86405958684218</v>
+        <v>0.15862657975318</v>
       </c>
       <c r="G40" t="n">
-        <v>0.000545153507843612</v>
+        <v>0.853449298766526</v>
       </c>
     </row>
     <row r="41">
@@ -5599,22 +5662,22 @@
         <v>81</v>
       </c>
       <c r="B41" t="n">
-        <v>1.65108317592598</v>
+        <v>5.76889793299689</v>
       </c>
       <c r="C41" t="n">
-        <v>0.825541587962989</v>
+        <v>2.88444896649845</v>
       </c>
       <c r="D41" t="n">
         <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>166.482583826741</v>
+        <v>165.431462258882</v>
       </c>
       <c r="F41" t="n">
-        <v>1.00164037053806</v>
+        <v>0.713957089894244</v>
       </c>
       <c r="G41" t="n">
-        <v>0.36947879630977</v>
+        <v>0.491205128149826</v>
       </c>
     </row>
     <row r="42">
@@ -5622,22 +5685,22 @@
         <v>82</v>
       </c>
       <c r="B42" t="n">
-        <v>3.0153280310987</v>
+        <v>3.23200732526919</v>
       </c>
       <c r="C42" t="n">
-        <v>1.50766401554935</v>
+        <v>3.23200732526919</v>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>168.347869865607</v>
+        <v>34.9640335888948</v>
       </c>
       <c r="F42" t="n">
-        <v>8.06888367539515</v>
+        <v>0.799984527813387</v>
       </c>
       <c r="G42" t="n">
-        <v>0.000450474987633068</v>
+        <v>0.377213938644727</v>
       </c>
     </row>
     <row r="43">
@@ -5645,21 +5708,504 @@
         <v>83</v>
       </c>
       <c r="B43" t="n">
-        <v>0.495573511079275</v>
+        <v>5.73612839020968</v>
       </c>
       <c r="C43" t="n">
-        <v>0.247786755539638</v>
+        <v>2.86806419510484</v>
       </c>
       <c r="D43" t="n">
         <v>2</v>
       </c>
       <c r="E43" t="n">
+        <v>165.431462267043</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.709901541039461</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.49318421114143</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.97257890977619</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.986289454888094</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>166.368454156484</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.265348731221794</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.767262409098309</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.763410649108322</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.763410649108322</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>37.3872827858006</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.205386001176585</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.653027485289988</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.775013488375225</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.387506744187613</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>166.368454153572</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.104253799328857</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.901055410980795</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="n">
+        <v>4.2644309719298</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2.1322154859649</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="n">
+        <v>166.999605964416</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.51921012405298</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.221894082947909</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.783019290709749</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.783019290709749</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>38.3311820537991</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.557903664805582</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.459663467724767</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.0408831236320545</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0204415618160272</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="n">
+        <v>166.999605970694</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.0145646759751911</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.985542127583754</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.65201519382752</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.82600759691376</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="n">
+        <v>167.381180361829</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4.34988215812931</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.0143988293435929</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.447473746931606</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.447473746931606</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="n">
+        <v>37.8185516528658</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2.35646509218762</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.133089253850407</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.24578226944085</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.122891134720425</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" t="n">
+        <v>167.381180362697</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.647163484101047</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.524833550797446</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" t="n">
+        <v>3.75470464974175</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1.87735232487088</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" t="n">
+        <v>166.749929210979</v>
+      </c>
+      <c r="F53" t="n">
+        <v>7.3342621111996</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.000885439303093956</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.163404168393309</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.163404168393309</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="n">
+        <v>37.2119050239365</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.638371916225984</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.429371364581734</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.0346290995055498</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0173145497527749</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" t="n">
+        <v>166.749929206417</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0676428417521424</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.934619843401819</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" t="n">
+        <v>8.45322707076706</v>
+      </c>
+      <c r="C56" t="n">
+        <v>4.22661353538353</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="n">
+        <v>167.121558215257</v>
+      </c>
+      <c r="F56" t="n">
+        <v>5.13473139839836</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.0068524559615141</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.36874594002769</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1.36874594002769</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>37.597045470648</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1.6628307026071</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.205098209146818</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.948644424324568</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.474322212162284</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="n">
+        <v>167.121558214899</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.576233699948733</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.563123711755617</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" t="n">
+        <v>12.962952433057</v>
+      </c>
+      <c r="C59" t="n">
+        <v>6.4814762165285</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" t="n">
+        <v>166.482583821998</v>
+      </c>
+      <c r="F59" t="n">
+        <v>7.86405958684218</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.000545153507843612</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.29285752677233</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1.29285752677233</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="n">
+        <v>37.48641953068</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1.568640891084</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.218162067140755</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.65108317592598</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.825541587962989</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="n">
+        <v>166.482583826741</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1.00164037053806</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.36947879630977</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" t="n">
+        <v>3.0153280310987</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1.50766401554935</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>168.347869865607</v>
+      </c>
+      <c r="F62" t="n">
+        <v>8.06888367539515</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.000450474987633068</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.239155892628385</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.239155892628385</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="n">
+        <v>38.6783582304257</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1.27994105981272</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.264876031959553</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.495573511079275</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.247786755539638</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" t="n">
         <v>168.347869865644</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F64" t="n">
         <v>1.32613267023184</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G64" t="n">
         <v>0.268261046767134</v>
       </c>
     </row>

</xml_diff>